<commit_message>
calculation of missing nutritional content with conversion rates
</commit_message>
<xml_diff>
--- a/CleanedData.xlsx
+++ b/CleanedData.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Vitamins" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="VitaminCoverage" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,97 +435,77 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>food</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>food</t>
+          <t>A Retinol (µg)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>label</t>
+          <t>B1 Thiamin (µg)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>A Retinoläquivalent (µg)</t>
+          <t>B2 Riboflavin (µg)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>A Retinol (µg)</t>
+          <t>B3 Niacin, Nicotinsäure (µg)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>A Beta-Carotin (µg)</t>
+          <t>B5 Pantothensäure (µg)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>B1 Thiamin (µg)</t>
+          <t>B6 Pyridoxin (µg)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>B2 Riboflavin (µg)</t>
+          <t>B7 Biotin (Vitamin H) (µg)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>B3 Niacin, Nicotinsäure (µg)</t>
+          <t>B9 gesamte Folsäure (µg)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>B3 Niacinäquivalent (µg)</t>
+          <t>B12 Cobalamin (µg)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>B5 Pantothensäure (µg)</t>
+          <t>C Ascorbinsäure (µg)</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>B6 Pyridoxin (µg)</t>
+          <t>D Calciferole (µg)</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>B7 Biotin (Vitamin H) (µg)</t>
+          <t>E Tocopherole (µg)</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>B9 gesamte Folsäure (µg)</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>B12 Cobalamin (µg)</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>C Ascorbinsäure (µg)</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>D Calciferole (µg)</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>E Tocopherole (µg)</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>K (µg)</t>
         </is>
@@ -534,65 +515,48 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Banane</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>BANANE FRISCH</t>
-        </is>
+      <c r="C2" t="n">
+        <v>57.2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44</v>
       </c>
       <c r="E2" t="n">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>838.2</v>
       </c>
       <c r="G2" t="n">
         <v>230</v>
       </c>
       <c r="H2" t="n">
-        <v>44</v>
+        <v>370</v>
       </c>
       <c r="I2" t="n">
-        <v>57</v>
+        <v>5.5</v>
       </c>
       <c r="J2" t="n">
-        <v>650</v>
+        <v>20</v>
       </c>
       <c r="K2" t="n">
-        <v>950</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>230</v>
+        <v>12000</v>
       </c>
       <c r="M2" t="n">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>5.5</v>
+        <v>270</v>
       </c>
       <c r="O2" t="n">
-        <v>20</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>12000</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>270</v>
-      </c>
-      <c r="T2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -600,65 +564,48 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Brennessel</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>BRENNNESSEL ROH</t>
-        </is>
+      <c r="C3" t="n">
+        <v>600</v>
+      </c>
+      <c r="D3" t="n">
+        <v>200</v>
       </c>
       <c r="E3" t="n">
-        <v>400</v>
+        <v>150</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>3293.8</v>
       </c>
       <c r="G3" t="n">
-        <v>2400</v>
+        <v>300</v>
       </c>
       <c r="H3" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="I3" t="n">
-        <v>150</v>
+        <v>0.5</v>
       </c>
       <c r="J3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>333000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
         <v>800</v>
       </c>
-      <c r="K3" t="n">
-        <v>3733</v>
-      </c>
-      <c r="L3" t="n">
-        <v>300</v>
-      </c>
-      <c r="M3" t="n">
-        <v>160</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.5</v>
-      </c>
       <c r="O3" t="n">
-        <v>30</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>333000</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>800</v>
-      </c>
-      <c r="T3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -666,65 +613,48 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Broccoli</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>BROCCOLI FRISCH</t>
-        </is>
+      <c r="C4" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>98</v>
       </c>
       <c r="E4" t="n">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1367.6</v>
       </c>
       <c r="G4" t="n">
-        <v>846</v>
+        <v>1290</v>
       </c>
       <c r="H4" t="n">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="I4" t="n">
-        <v>178</v>
+        <v>0.5</v>
       </c>
       <c r="J4" t="n">
-        <v>1000</v>
+        <v>90</v>
       </c>
       <c r="K4" t="n">
-        <v>1550</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1290</v>
+        <v>115000</v>
       </c>
       <c r="M4" t="n">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0.5</v>
+        <v>621</v>
       </c>
       <c r="O4" t="n">
-        <v>90</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>115000</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
-        <v>621</v>
-      </c>
-      <c r="T4" t="n">
         <v>121</v>
       </c>
     </row>
@@ -732,65 +662,48 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Kakao</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>KAKAOBOHNE, -MASSE</t>
-        </is>
+      <c r="C5" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>130</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>400</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>5882.6</v>
       </c>
       <c r="G5" t="n">
-        <v>40</v>
+        <v>1100</v>
       </c>
       <c r="H5" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="I5" t="n">
-        <v>400</v>
+        <v>20</v>
       </c>
       <c r="J5" t="n">
-        <v>2700</v>
+        <v>38</v>
       </c>
       <c r="K5" t="n">
-        <v>6667</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>20</v>
+        <v>680</v>
       </c>
       <c r="O5" t="n">
-        <v>38</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>680</v>
-      </c>
-      <c r="T5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -798,65 +711,48 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Rinderhackfleisch</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>RIND HACKFLEISCH FRISCH</t>
-        </is>
+      <c r="C6" t="n">
+        <v>17</v>
+      </c>
+      <c r="D6" t="n">
+        <v>198</v>
       </c>
       <c r="E6" t="n">
-        <v>17</v>
+        <v>228</v>
       </c>
       <c r="F6" t="n">
-        <v>17</v>
+        <v>8881.799999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>498</v>
       </c>
       <c r="H6" t="n">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="I6" t="n">
-        <v>228</v>
+        <v>2.5</v>
       </c>
       <c r="J6" t="n">
-        <v>6466</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>10066</v>
+        <v>4.4</v>
       </c>
       <c r="L6" t="n">
-        <v>498</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>2.5</v>
+        <v>398</v>
       </c>
       <c r="O6" t="n">
-        <v>2</v>
-      </c>
-      <c r="P6" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" t="n">
-        <v>398</v>
-      </c>
-      <c r="T6" t="n">
         <v>11</v>
       </c>
     </row>
@@ -864,65 +760,48 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>Rinderleber</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>RIND LEBER ROH</t>
-        </is>
+      <c r="C7" t="n">
+        <v>17900</v>
+      </c>
+      <c r="D7" t="n">
+        <v>266</v>
       </c>
       <c r="E7" t="n">
-        <v>17900</v>
+        <v>3085</v>
       </c>
       <c r="F7" t="n">
-        <v>17900</v>
+        <v>17529.7</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>7300</v>
       </c>
       <c r="H7" t="n">
-        <v>266</v>
+        <v>961</v>
       </c>
       <c r="I7" t="n">
-        <v>3085</v>
+        <v>100</v>
       </c>
       <c r="J7" t="n">
-        <v>14700</v>
+        <v>592</v>
       </c>
       <c r="K7" t="n">
-        <v>19867</v>
+        <v>65</v>
       </c>
       <c r="L7" t="n">
-        <v>7300</v>
+        <v>32000</v>
       </c>
       <c r="M7" t="n">
-        <v>961</v>
+        <v>1.7</v>
       </c>
       <c r="N7" t="n">
-        <v>100</v>
+        <v>750</v>
       </c>
       <c r="O7" t="n">
-        <v>592</v>
-      </c>
-      <c r="P7" t="n">
-        <v>65</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>32000</v>
-      </c>
-      <c r="R7" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="S7" t="n">
-        <v>750</v>
-      </c>
-      <c r="T7" t="n">
         <v>75</v>
       </c>
     </row>
@@ -930,65 +809,48 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>Makrele</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>MAKRELE ROH FISCHZUSCHNITT</t>
-        </is>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>130</v>
       </c>
       <c r="E8" t="n">
-        <v>100</v>
+        <v>360</v>
       </c>
       <c r="F8" t="n">
-        <v>100</v>
+        <v>10588.2</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>460</v>
       </c>
       <c r="H8" t="n">
-        <v>130</v>
+        <v>630</v>
       </c>
       <c r="I8" t="n">
-        <v>360</v>
+        <v>4</v>
       </c>
       <c r="J8" t="n">
-        <v>7500</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>12000</v>
+        <v>9</v>
       </c>
       <c r="L8" t="n">
-        <v>460</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>630</v>
+        <v>4</v>
       </c>
       <c r="N8" t="n">
-        <v>4</v>
+        <v>1250</v>
       </c>
       <c r="O8" t="n">
-        <v>1</v>
-      </c>
-      <c r="P8" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>4</v>
-      </c>
-      <c r="S8" t="n">
-        <v>1250</v>
-      </c>
-      <c r="T8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -996,65 +858,48 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Haferflocken</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>HAFERFLOCKEN</t>
-        </is>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>562</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>3676.8</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1090</v>
       </c>
       <c r="H9" t="n">
-        <v>562</v>
+        <v>98</v>
       </c>
       <c r="I9" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J9" t="n">
-        <v>1000</v>
+        <v>87</v>
       </c>
       <c r="K9" t="n">
-        <v>4167</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>1090</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>20</v>
+        <v>800</v>
       </c>
       <c r="O9" t="n">
-        <v>87</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" t="n">
-        <v>800</v>
-      </c>
-      <c r="T9" t="n">
         <v>63</v>
       </c>
     </row>
@@ -1062,65 +907,48 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>8</v>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Kefir</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>KEFIR</t>
-        </is>
+      <c r="C10" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>40</v>
       </c>
       <c r="E10" t="n">
-        <v>22</v>
+        <v>170</v>
       </c>
       <c r="F10" t="n">
-        <v>20</v>
+        <v>726.2</v>
       </c>
       <c r="G10" t="n">
-        <v>10</v>
+        <v>370</v>
       </c>
       <c r="H10" t="n">
+        <v>50</v>
+      </c>
+      <c r="I10" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J10" t="n">
+        <v>5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
         <v>40</v>
       </c>
-      <c r="I10" t="n">
-        <v>170</v>
-      </c>
-      <c r="J10" t="n">
-        <v>90</v>
-      </c>
-      <c r="K10" t="n">
-        <v>823</v>
-      </c>
-      <c r="L10" t="n">
-        <v>370</v>
-      </c>
-      <c r="M10" t="n">
-        <v>50</v>
-      </c>
-      <c r="N10" t="n">
-        <v>3.6</v>
-      </c>
       <c r="O10" t="n">
-        <v>5</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>1000</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" t="n">
-        <v>40</v>
-      </c>
-      <c r="T10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1128,65 +956,48 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
-        <v>9</v>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Walnüsse</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>WALNÜSSE</t>
-        </is>
+      <c r="C11" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" t="n">
+        <v>340</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>2794.4</v>
       </c>
       <c r="G11" t="n">
-        <v>48</v>
+        <v>820</v>
       </c>
       <c r="H11" t="n">
-        <v>340</v>
+        <v>870</v>
       </c>
       <c r="I11" t="n">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="J11" t="n">
-        <v>1000</v>
+        <v>77</v>
       </c>
       <c r="K11" t="n">
-        <v>3167</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>820</v>
+        <v>2600</v>
       </c>
       <c r="M11" t="n">
-        <v>870</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>19</v>
+        <v>6040</v>
       </c>
       <c r="O11" t="n">
-        <v>77</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>2600</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" t="n">
-        <v>6040</v>
-      </c>
-      <c r="T11" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1194,66 +1005,684 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Vollei</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>277.1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>100</v>
+      </c>
+      <c r="E12" t="n">
+        <v>310</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2735.3</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1600</v>
+      </c>
+      <c r="H12" t="n">
+        <v>120</v>
+      </c>
+      <c r="I12" t="n">
+        <v>25</v>
+      </c>
+      <c r="J12" t="n">
+        <v>65</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2022</v>
+      </c>
+      <c r="O12" t="n">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>B5</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>B9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>B12</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Banane</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5.72</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5.59</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="I2" t="n">
+        <v>12.22</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>12</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="O2" t="n">
+        <v>15.38</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Brennessel</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>60</v>
+      </c>
+      <c r="D3" t="n">
+        <v>18.18</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>21.96</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>333</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Broccoli</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>21.35</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8.91</v>
+      </c>
+      <c r="E4" t="n">
+        <v>14.83</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9.119999999999999</v>
+      </c>
+      <c r="G4" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="J4" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>115</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="O4" t="n">
+        <v>186.15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Kakao</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11.82</v>
+      </c>
+      <c r="E5" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="F5" t="n">
+        <v>39.22</v>
+      </c>
+      <c r="G5" t="n">
+        <v>18.33</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="I5" t="n">
+        <v>44.44</v>
+      </c>
+      <c r="J5" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rinderhackfleisch</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E6" t="n">
+        <v>19</v>
+      </c>
+      <c r="F6" t="n">
+        <v>59.21</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>110</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="O6" t="n">
+        <v>16.92</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Rinderleber</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1790</v>
+      </c>
+      <c r="D7" t="n">
+        <v>24.18</v>
+      </c>
+      <c r="E7" t="n">
+        <v>257.08</v>
+      </c>
+      <c r="F7" t="n">
+        <v>116.86</v>
+      </c>
+      <c r="G7" t="n">
+        <v>121.67</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6.01</v>
+      </c>
+      <c r="I7" t="n">
+        <v>222.22</v>
+      </c>
+      <c r="J7" t="n">
+        <v>148</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1625</v>
+      </c>
+      <c r="L7" t="n">
+        <v>32</v>
+      </c>
+      <c r="M7" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>5.36</v>
+      </c>
+      <c r="O7" t="n">
+        <v>115.38</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Makrele</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>10</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D8" t="n">
+        <v>11.82</v>
+      </c>
+      <c r="E8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F8" t="n">
+        <v>70.59</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7.67</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="I8" t="n">
+        <v>8.890000000000001</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K8" t="n">
+        <v>225</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>20</v>
+      </c>
+      <c r="N8" t="n">
+        <v>8.93</v>
+      </c>
+      <c r="O8" t="n">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Haferflocken</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>51.09</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="F9" t="n">
+        <v>24.51</v>
+      </c>
+      <c r="G9" t="n">
+        <v>18.17</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="I9" t="n">
+        <v>44.44</v>
+      </c>
+      <c r="J9" t="n">
+        <v>21.75</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="O9" t="n">
+        <v>96.92</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Kefir</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="E10" t="n">
+        <v>14.17</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.84</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="I10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="K10" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="O10" t="n">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Walnüsse</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>30.91</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="n">
+        <v>18.63</v>
+      </c>
+      <c r="G11" t="n">
+        <v>13.67</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5.44</v>
+      </c>
+      <c r="I11" t="n">
+        <v>42.22</v>
+      </c>
+      <c r="J11" t="n">
+        <v>19.25</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>43.14</v>
+      </c>
+      <c r="O11" t="n">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Vollei</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>HÜHNEREI VOLLEI</t>
-        </is>
+      <c r="C12" t="n">
+        <v>27.71</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9.09</v>
       </c>
       <c r="E12" t="n">
-        <v>278</v>
+        <v>25.83</v>
       </c>
       <c r="F12" t="n">
-        <v>276</v>
+        <v>18.24</v>
       </c>
       <c r="G12" t="n">
-        <v>13</v>
+        <v>26.67</v>
       </c>
       <c r="H12" t="n">
-        <v>100</v>
+        <v>0.75</v>
       </c>
       <c r="I12" t="n">
-        <v>310</v>
+        <v>55.56</v>
       </c>
       <c r="J12" t="n">
-        <v>83</v>
+        <v>16.25</v>
       </c>
       <c r="K12" t="n">
-        <v>3100</v>
+        <v>50</v>
       </c>
       <c r="L12" t="n">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>120</v>
+        <v>14.5</v>
       </c>
       <c r="N12" t="n">
-        <v>25</v>
+        <v>14.44</v>
       </c>
       <c r="O12" t="n">
-        <v>65</v>
-      </c>
-      <c r="P12" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="S12" t="n">
-        <v>2022</v>
-      </c>
-      <c r="T12" t="n">
-        <v>48</v>
+        <v>73.84999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>